<commit_message>
Tests: updated all tests
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model4.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="106">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -630,14 +630,14 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.5182186234818"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.1619433198381"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -769,14 +769,14 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
+      <selection pane="topLeft" activeCell="L31" activeCellId="1" sqref="A:D L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -913,7 +913,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1147,10 +1147,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.99</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.99</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.99</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.99</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.99</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -1356,7 +1356,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -1370,7 +1370,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.99</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.99</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.99</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.99</v>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.99</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.99</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.99</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.99</v>
@@ -1491,6 +1491,34 @@
         <v>1</v>
       </c>
       <c r="D24" s="0" t="n">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="0" t="n">
         <v>1.01</v>
       </c>
     </row>
@@ -1513,14 +1541,14 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.46153846153846"/>
   </cols>
@@ -1811,12 +1839,12 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
@@ -3039,7 +3067,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3586,7 +3614,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3826,7 +3854,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3928,7 +3956,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4085,7 +4113,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4242,13 +4270,13 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.46153846153846"/>
   </cols>
@@ -4437,7 +4465,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Feat: removed dependency on mets active and fixed cols
metsActive are now metsBalanced if only reference
state or one condition; they are mets that change
across conditions if more than one condition.
metsFixed are the complement of metsBalanced
if only reference state or one condition; they
are the mets that do not change over conditions
if more than one condition.
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model4.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -640,8 +640,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -787,7 +787,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L31" activeCellId="1" sqref="A5:B5 L31"/>
+      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,7 +931,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5:B5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A5:B5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1559,13 +1559,13 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="1" sqref="A5:B5 B39"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.46"/>
@@ -1857,7 +1857,7 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5:B5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3084,8 +3084,8 @@
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="A5:B5 D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3127,7 +3127,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
@@ -3167,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
@@ -3227,7 +3227,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0</v>
@@ -3367,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>0</v>
@@ -3407,7 +3407,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>0</v>
@@ -3447,7 +3447,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>0</v>
@@ -3467,7 +3467,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>0</v>
@@ -3587,7 +3587,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>0</v>
@@ -3607,7 +3607,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
@@ -3632,7 +3632,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="A5:B5 C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3872,7 +3872,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5:B5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3974,7 +3974,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5:B5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4131,7 +4131,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5:B5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4288,7 +4288,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5:B5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4483,7 +4483,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A5:B5 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>